<commit_message>
created tests so that part III is finished and ready for submission
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="34">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -103,19 +103,25 @@
     <t xml:space="preserve">White: Door Direction Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">Orange: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purple: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Purple:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Blue:</t>
+    <t xml:space="preserve">Orange: locations  within rooms adjacency test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purple: adjacency list should include doorway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green: walkway only tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Purple: locations at each edge of the board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pink: targets along walkways at various distances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light Blue: targets that allow the user to enter a room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Orange: targets calculated when leaving a room</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +176,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA1467E"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
@@ -182,8 +194,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF3F00"/>
+        <bgColor rgb="FFFF3838"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4E102D"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81ACA6"/>
+        <bgColor rgb="FF9999FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF3838"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF127622"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000358"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFFF3F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -221,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,11 +292,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,7 +304,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,18 +360,18 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF127622"/>
+      <rgbColor rgb="FF000358"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFA1467E"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FF4E102D"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
@@ -309,16 +395,16 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF3F00"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF81ACA6"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
@@ -331,10 +417,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +470,7 @@
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -411,7 +497,7 @@
       <c r="V1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="X1" s="1" t="s">
@@ -420,7 +506,7 @@
       <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="4" t="n">
+      <c r="Z1" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -491,7 +577,7 @@
       <c r="V2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -500,7 +586,7 @@
       <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="4" t="n">
+      <c r="Z2" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -580,7 +666,7 @@
       <c r="Y3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="4" t="n">
+      <c r="Z3" s="5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -612,10 +698,10 @@
       <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -633,7 +719,7 @@
       <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -660,7 +746,7 @@
       <c r="Y4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="4" t="n">
+      <c r="Z4" s="5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -674,7 +760,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -695,7 +781,7 @@
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -740,7 +826,7 @@
       <c r="Y5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z5" s="4" t="n">
+      <c r="Z5" s="5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -793,7 +879,7 @@
       <c r="P6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -820,7 +906,7 @@
       <c r="Y6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="4" t="n">
+      <c r="Z6" s="5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -900,7 +986,7 @@
       <c r="Y7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z7" s="4" t="n">
+      <c r="Z7" s="5" t="n">
         <v>6</v>
       </c>
     </row>
@@ -908,7 +994,7 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -980,7 +1066,7 @@
       <c r="Y8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="4" t="n">
+      <c r="Z8" s="5" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1003,37 +1089,37 @@
       <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="6" t="s">
+      <c r="I9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="2" t="s">
@@ -1060,7 +1146,7 @@
       <c r="Y9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z9" s="4" t="n">
+      <c r="Z9" s="5" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1077,7 +1163,7 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1089,31 +1175,31 @@
       <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="6" t="s">
+      <c r="I10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -1125,7 +1211,7 @@
       <c r="T10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="U10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="V10" s="1" t="s">
@@ -1140,7 +1226,7 @@
       <c r="Y10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z10" s="4" t="n">
+      <c r="Z10" s="5" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1157,10 +1243,10 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1169,31 +1255,31 @@
       <c r="H11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q11" s="6" t="s">
+      <c r="I11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R11" s="2" t="s">
@@ -1220,7 +1306,7 @@
       <c r="Y11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="4" t="n">
+      <c r="Z11" s="5" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1249,31 +1335,31 @@
       <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12" s="6" t="s">
+      <c r="I12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -1300,7 +1386,7 @@
       <c r="Y12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z12" s="4" t="n">
+      <c r="Z12" s="5" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1329,31 +1415,31 @@
       <c r="H13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="6" t="s">
+      <c r="I13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -1374,18 +1460,18 @@
       <c r="W13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="3" t="s">
+      <c r="X13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="4" t="n">
+      <c r="Z13" s="5" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1409,31 +1495,31 @@
       <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q14" s="6" t="s">
+      <c r="I14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -1460,7 +1546,7 @@
       <c r="Y14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z14" s="4" t="n">
+      <c r="Z14" s="5" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1489,31 +1575,31 @@
       <c r="H15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="6" t="s">
+      <c r="I15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="10" t="s">
         <v>11</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1534,13 +1620,13 @@
       <c r="W15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X15" s="3" t="s">
+      <c r="X15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Y15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="4" t="n">
+      <c r="Z15" s="5" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1620,7 +1706,7 @@
       <c r="Y16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z16" s="4" t="n">
+      <c r="Z16" s="5" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1661,7 +1747,7 @@
       <c r="L17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="11" t="s">
         <v>1</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -1700,7 +1786,7 @@
       <c r="Y17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z17" s="4" t="n">
+      <c r="Z17" s="5" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1711,7 +1797,7 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1759,7 +1845,7 @@
       <c r="R18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="S18" s="12" t="s">
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
@@ -1777,10 +1863,10 @@
       <c r="X18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="4" t="n">
+      <c r="Y18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="5" t="n">
         <v>17</v>
       </c>
     </row>
@@ -1791,7 +1877,7 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1812,7 +1898,7 @@
       <c r="I19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="12" t="s">
         <v>1</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1824,7 +1910,7 @@
       <c r="M19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="13" t="s">
         <v>1</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -1860,7 +1946,7 @@
       <c r="Y19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z19" s="4" t="n">
+      <c r="Z19" s="5" t="n">
         <v>18</v>
       </c>
     </row>
@@ -1931,7 +2017,7 @@
       <c r="V20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="3" t="s">
+      <c r="W20" s="4" t="s">
         <v>20</v>
       </c>
       <c r="X20" s="1" t="s">
@@ -1940,7 +2026,7 @@
       <c r="Y20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z20" s="4" t="n">
+      <c r="Z20" s="5" t="n">
         <v>19</v>
       </c>
     </row>
@@ -1963,10 +2049,10 @@
       <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="5" t="s">
+      <c r="G21" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2020,7 +2106,7 @@
       <c r="Y21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z21" s="4" t="n">
+      <c r="Z21" s="5" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2100,7 +2186,7 @@
       <c r="Y22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z22" s="4" t="n">
+      <c r="Z22" s="5" t="n">
         <v>21</v>
       </c>
     </row>
@@ -2114,7 +2200,7 @@
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -2135,7 +2221,7 @@
       <c r="J23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -2159,7 +2245,7 @@
       <c r="R23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="3" t="s">
+      <c r="S23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T23" s="1" t="s">
@@ -2168,7 +2254,7 @@
       <c r="U23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="V23" s="14" t="s">
         <v>18</v>
       </c>
       <c r="W23" s="1" t="s">
@@ -2180,7 +2266,7 @@
       <c r="Y23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z23" s="4" t="n">
+      <c r="Z23" s="5" t="n">
         <v>22</v>
       </c>
     </row>
@@ -2260,7 +2346,7 @@
       <c r="Y24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z24" s="4" t="n">
+      <c r="Z24" s="5" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2307,7 +2393,7 @@
       <c r="N25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="O25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P25" s="2" t="s">
@@ -2340,185 +2426,195 @@
       <c r="Y25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z25" s="4" t="n">
+      <c r="Z25" s="5" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="n">
+      <c r="A26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="n">
+      <c r="B26" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G26" s="4" t="n">
+      <c r="F26" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="J26" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K26" s="4" t="n">
+      <c r="J26" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K26" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="L26" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="M26" s="4" t="n">
+      <c r="L26" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M26" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="N26" s="4" t="n">
+      <c r="N26" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="O26" s="4" t="n">
+      <c r="O26" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="P26" s="4" t="n">
+      <c r="P26" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="Q26" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="R26" s="4" t="n">
+      <c r="Q26" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="R26" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="S26" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="T26" s="4" t="n">
+      <c r="S26" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="T26" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="U26" s="4" t="n">
+      <c r="U26" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="V26" s="4" t="n">
+      <c r="V26" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="W26" s="4" t="n">
+      <c r="W26" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="X26" s="4" t="n">
+      <c r="X26" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="Y26" s="4" t="n">
+      <c r="Y26" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="Z26" s="4"/>
+      <c r="Z26" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Finished implementation of calcAdjacencies and calcTargets and all tests pass
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\Eclipse-Workspace\ClueGame\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6030" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,118 +24,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="34">
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of doors: 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White: Door Direction Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orange: locations  within rooms adjacency test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purple: adjacency list should include doorway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green: walkway only tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Purple: locations at each edge of the board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pink: targets along walkways at various distances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light Blue: targets that allow the user to enter a room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dark Orange: targets calculated when leaving a room</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="36">
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>Number of doors: 18</t>
+  </si>
+  <si>
+    <t>White: Door Direction Tests</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list should include doorway</t>
+  </si>
+  <si>
+    <t>Green: walkway only tests</t>
+  </si>
+  <si>
+    <t>Light Purple: locations at each edge of the board</t>
+  </si>
+  <si>
+    <t>Pink: targets along walkways at various distances</t>
+  </si>
+  <si>
+    <t>Light Blue: targets that allow the user to enter a room</t>
+  </si>
+  <si>
+    <t>Dark Orange: targets calculated when leaving a room</t>
+  </si>
+  <si>
+    <t>Light Orange: locations  within rooms adjacency test</t>
+  </si>
+  <si>
+    <t>Dark Blue: Locations that are beside a room cell that is not a doorway</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,23 +146,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +168,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA1467E"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
@@ -190,18 +176,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3F00"/>
-        <bgColor rgb="FFFF3838"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4E102D"/>
-        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
@@ -218,137 +192,260 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF127622"/>
+        <fgColor theme="5"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000358"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6969"/>
+        <bgColor rgb="FFFF3F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6969"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF990099"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF990099"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor rgb="FF000080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3838"/>
-        <bgColor rgb="FFFF3F00"/>
+        <fgColor rgb="FF996633"/>
+        <bgColor rgb="FFFF3838"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF8080"/>
+        <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="5">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -407,30 +504,309 @@
       <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF996633"/>
+      <color rgb="FF990099"/>
+      <color rgb="FFFF6969"/>
+    </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Z36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="1" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="4.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="3.66"/>
+    <col min="1" max="24" width="4" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" customWidth="1"/>
+    <col min="26" max="26" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +846,7 @@
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -497,7 +873,7 @@
       <c r="V1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X1" s="1" t="s">
@@ -506,11 +882,11 @@
       <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="5" t="n">
+      <c r="Z1" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +953,7 @@
       <c r="V2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="X2" s="1" t="s">
@@ -586,11 +962,11 @@
       <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,11 +1042,11 @@
       <c r="Y3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="5" t="n">
+      <c r="Z3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,10 +1074,10 @@
       <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -719,7 +1095,7 @@
       <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -746,11 +1122,11 @@
       <c r="Y4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="5" t="n">
+      <c r="Z4" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +1136,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -781,7 +1157,7 @@
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -826,11 +1202,11 @@
       <c r="Y5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z5" s="5" t="n">
+      <c r="Z5" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -879,7 +1255,7 @@
       <c r="P6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -906,11 +1282,11 @@
       <c r="Y6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -986,15 +1362,15 @@
       <c r="Y7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z7" s="5" t="n">
+      <c r="Z7" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1066,11 +1442,11 @@
       <c r="Y8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="5" t="n">
+      <c r="Z8" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1089,37 +1465,37 @@
       <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="10" t="s">
+      <c r="I9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="2" t="s">
@@ -1146,11 +1522,11 @@
       <c r="Y9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z9" s="5" t="n">
+      <c r="Z9" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1539,7 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1175,31 +1551,31 @@
       <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="10" t="s">
+      <c r="I10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -1211,7 +1587,7 @@
       <c r="T10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="U10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="V10" s="1" t="s">
@@ -1226,11 +1602,11 @@
       <c r="Y10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z10" s="5" t="n">
+      <c r="Z10" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1243,10 +1619,10 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="14" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1255,31 +1631,31 @@
       <c r="H11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q11" s="10" t="s">
+      <c r="I11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R11" s="2" t="s">
@@ -1306,11 +1682,11 @@
       <c r="Y11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z11" s="5" t="n">
+      <c r="Z11" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1335,31 +1711,31 @@
       <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12" s="10" t="s">
+      <c r="I12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -1386,11 +1762,11 @@
       <c r="Y12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z12" s="5" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z12" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1415,31 +1791,31 @@
       <c r="H13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="10" t="s">
+      <c r="I13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -1460,18 +1836,18 @@
       <c r="W13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="7" t="s">
+      <c r="X13" s="17" t="s">
         <v>14</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="5" t="n">
+      <c r="Z13" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1495,31 +1871,31 @@
       <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q14" s="10" t="s">
+      <c r="I14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -1546,11 +1922,11 @@
       <c r="Y14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z14" s="5" t="n">
+      <c r="Z14" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1575,31 +1951,31 @@
       <c r="H15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="10" t="s">
+      <c r="I15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1620,17 +1996,17 @@
       <c r="W15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Y15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="5" t="n">
+      <c r="Z15" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1706,11 +2082,11 @@
       <c r="Y16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z16" s="5" t="n">
+      <c r="Z16" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +2123,7 @@
       <c r="L17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -1786,18 +2162,18 @@
       <c r="Y17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z17" s="5" t="n">
+      <c r="Z17" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1845,7 +2221,7 @@
       <c r="R18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="12" t="s">
+      <c r="S18" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
@@ -1863,21 +2239,21 @@
       <c r="X18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="5" t="n">
+      <c r="Y18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1898,7 +2274,7 @@
       <c r="I19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1946,11 +2322,11 @@
       <c r="Y19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z19" s="5" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z19" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2017,7 +2393,7 @@
       <c r="V20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="4" t="s">
+      <c r="W20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="X20" s="1" t="s">
@@ -2026,11 +2402,11 @@
       <c r="Y20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z20" s="5" t="n">
+      <c r="Z20" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2049,10 +2425,10 @@
       <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="G21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2106,11 +2482,11 @@
       <c r="Y21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z21" s="5" t="n">
+      <c r="Z21" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -2186,11 +2562,11 @@
       <c r="Y22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z22" s="5" t="n">
+      <c r="Z22" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -2200,7 +2576,7 @@
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -2221,7 +2597,7 @@
       <c r="J23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -2245,7 +2621,7 @@
       <c r="R23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="T23" s="1" t="s">
@@ -2254,7 +2630,7 @@
       <c r="U23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="V23" s="11" t="s">
         <v>18</v>
       </c>
       <c r="W23" s="1" t="s">
@@ -2266,11 +2642,11 @@
       <c r="Y23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z23" s="5" t="n">
+      <c r="Z23" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2346,11 +2722,11 @@
       <c r="Y24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z24" s="5" t="n">
+      <c r="Z24" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2393,7 +2769,7 @@
       <c r="N25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="15" t="s">
         <v>1</v>
       </c>
       <c r="P25" s="2" t="s">
@@ -2426,212 +2802,334 @@
       <c r="Y25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z25" s="5" t="n">
+      <c r="Z25" s="4">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>0</v>
       </c>
-      <c r="B26" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="n">
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
         <v>2</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" s="4">
         <v>3</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" s="4">
         <v>4</v>
       </c>
-      <c r="F26" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G26" s="5" t="n">
+      <c r="F26" s="4">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4">
         <v>6</v>
       </c>
-      <c r="H26" s="5" t="n">
+      <c r="H26" s="4">
         <v>7</v>
       </c>
-      <c r="I26" s="5" t="n">
+      <c r="I26" s="4">
         <v>8</v>
       </c>
-      <c r="J26" s="5" t="n">
+      <c r="J26" s="4">
         <v>9</v>
       </c>
-      <c r="K26" s="5" t="n">
+      <c r="K26" s="4">
         <v>10</v>
       </c>
-      <c r="L26" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="M26" s="5" t="n">
+      <c r="L26" s="4">
+        <v>11</v>
+      </c>
+      <c r="M26" s="4">
         <v>12</v>
       </c>
-      <c r="N26" s="5" t="n">
+      <c r="N26" s="4">
         <v>13</v>
       </c>
-      <c r="O26" s="5" t="n">
+      <c r="O26" s="4">
         <v>14</v>
       </c>
-      <c r="P26" s="5" t="n">
+      <c r="P26" s="4">
         <v>15</v>
       </c>
-      <c r="Q26" s="5" t="n">
+      <c r="Q26" s="4">
         <v>16</v>
       </c>
-      <c r="R26" s="5" t="n">
+      <c r="R26" s="4">
         <v>17</v>
       </c>
-      <c r="S26" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="T26" s="5" t="n">
+      <c r="S26" s="4">
+        <v>18</v>
+      </c>
+      <c r="T26" s="4">
         <v>19</v>
       </c>
-      <c r="U26" s="5" t="n">
+      <c r="U26" s="4">
         <v>20</v>
       </c>
-      <c r="V26" s="5" t="n">
+      <c r="V26" s="4">
         <v>21</v>
       </c>
-      <c r="W26" s="5" t="n">
+      <c r="W26" s="4">
         <v>22</v>
       </c>
-      <c r="X26" s="5" t="n">
+      <c r="X26" s="4">
         <v>23</v>
       </c>
-      <c r="Y26" s="5" t="n">
+      <c r="Y26" s="4">
         <v>24</v>
       </c>
-      <c r="Z26" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="Z26" s="4"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" s="26"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>33</v>
-      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A32:J32"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:J34"/>
+  <mergeCells count="20">
+    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="A36:P36"/>
+    <mergeCell ref="A37:P37"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="A31:P31"/>
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="A32:P32"/>
+    <mergeCell ref="A33:P33"/>
+    <mergeCell ref="A34:P34"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created skeleton classes and test. I also added .txt files with the proper cards and people
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\Eclipse-Workspace\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsanc\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7920CC51-B23E-4931-BE8A-E500D71911A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6030" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="52">
   <si>
     <t>K</t>
   </si>
@@ -132,15 +133,70 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mrs. White</t>
+  </si>
+  <si>
+    <t>Mr. Green</t>
+  </si>
+  <si>
+    <t>Mrs. Peacock</t>
+  </si>
+  <si>
+    <t>Professor Plum</t>
+  </si>
+  <si>
+    <t>Miss Scarlett</t>
+  </si>
+  <si>
+    <t>Colonel Mustard</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Col</t>
+  </si>
+  <si>
+    <t>Character Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -287,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -347,11 +403,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -374,15 +439,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,6 +459,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,9 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -439,6 +501,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,21 +870,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="24" width="4" customWidth="1"/>
-    <col min="25" max="25" width="4.140625" customWidth="1"/>
-    <col min="26" max="26" width="3.7109375" customWidth="1"/>
+    <col min="25" max="25" width="4.109375" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +924,7 @@
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -886,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1214,7 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1157,7 +1235,7 @@
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1206,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1446,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1526,7 +1604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1606,7 +1684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1622,7 +1700,7 @@
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="11" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1686,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1766,7 +1844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1914,7 @@
       <c r="W13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="17" t="s">
+      <c r="X13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="Y13" s="1" t="s">
@@ -1846,8 +1924,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1926,7 +2004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -2086,7 +2164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2201,7 @@
       <c r="L17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="M17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -2166,14 +2244,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2221,7 +2299,7 @@
       <c r="R18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="16" t="s">
+      <c r="S18" s="13" t="s">
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
@@ -2239,14 +2317,14 @@
       <c r="X18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y18" s="15" t="s">
+      <c r="Y18" s="12" t="s">
         <v>1</v>
       </c>
       <c r="Z18" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2274,7 +2352,7 @@
       <c r="I19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="13" t="s">
         <v>1</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -2286,7 +2364,7 @@
       <c r="M19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="13" t="s">
+      <c r="N19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -2326,7 +2404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2406,7 +2484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2425,7 +2503,7 @@
       <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="11" t="s">
         <v>1</v>
       </c>
       <c r="H21" s="5" t="s">
@@ -2486,7 +2564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -2566,7 +2644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -2630,7 +2708,7 @@
       <c r="U23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V23" s="11" t="s">
+      <c r="V23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="W23" s="1" t="s">
@@ -2646,7 +2724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2726,7 +2804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2769,7 +2847,7 @@
       <c r="N25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="12" t="s">
         <v>1</v>
       </c>
       <c r="P25" s="2" t="s">
@@ -2806,7 +2884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>0</v>
       </c>
@@ -2884,230 +2962,371 @@
       </c>
       <c r="Z26" s="4"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="26" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="R28" s="26"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="R28" s="16"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="18"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
       <c r="Q32" s="20"/>
       <c r="R32" s="20"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
       <c r="Q33" s="21"/>
       <c r="R33" s="21"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
       <c r="Q35" s="23"/>
       <c r="R35" s="23"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
       <c r="Q36" s="24"/>
       <c r="R36" s="24"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
       <c r="Q37" s="25"/>
       <c r="R37" s="25"/>
     </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="30">
+        <v>24</v>
+      </c>
+      <c r="G41" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="33"/>
+      <c r="D42" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="32"/>
+      <c r="F42" s="30">
+        <v>24</v>
+      </c>
+      <c r="G42" s="30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="30">
+        <v>15</v>
+      </c>
+      <c r="G43" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="33"/>
+      <c r="D44" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="32"/>
+      <c r="F44" s="30">
+        <v>0</v>
+      </c>
+      <c r="G44" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="33"/>
+      <c r="D45" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="32"/>
+      <c r="F45" s="30">
+        <v>0</v>
+      </c>
+      <c r="G45" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="D46" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" s="32"/>
+      <c r="F46" s="30">
+        <v>18</v>
+      </c>
+      <c r="G46" s="30">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="35">
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="A32:P32"/>
+    <mergeCell ref="A33:P33"/>
+    <mergeCell ref="A34:P34"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B39:G39"/>
     <mergeCell ref="A35:P35"/>
     <mergeCell ref="A36:P36"/>
     <mergeCell ref="A37:P37"/>
@@ -3124,10 +3343,6 @@
     <mergeCell ref="A28:P28"/>
     <mergeCell ref="A29:P29"/>
     <mergeCell ref="A31:P31"/>
-    <mergeCell ref="A30:P30"/>
-    <mergeCell ref="A32:P32"/>
-    <mergeCell ref="A33:P33"/>
-    <mergeCell ref="A34:P34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added computer player target tests (failing)
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsanc\eclipse-workspace\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trent Douglas\OneDrive - Colorado School of Mines\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7920CC51-B23E-4931-BE8A-E500D71911A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,14 +460,30 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,22 +517,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,18 +873,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="24" width="4" customWidth="1"/>
-    <col min="25" max="25" width="4.109375" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" customWidth="1"/>
+    <col min="26" max="26" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>1</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>0</v>
       </c>
@@ -2962,239 +2962,239 @@
       </c>
       <c r="Z26" s="4"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="16" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="R28" s="16"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+      <c r="R28" s="23"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="29"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
-      <c r="O34" s="29"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B39" s="34" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="17" t="s">
         <v>36</v>
       </c>
@@ -3203,111 +3203,133 @@
         <v>35</v>
       </c>
       <c r="E40" s="17"/>
-      <c r="F40" s="30" t="s">
+      <c r="F40" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="31" t="s">
+    <row r="41" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="30">
+      <c r="E41" s="18"/>
+      <c r="F41" s="15">
         <v>24</v>
       </c>
-      <c r="G41" s="30">
+      <c r="G41" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="33" t="s">
+    <row r="42" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="32" t="s">
+      <c r="C42" s="16"/>
+      <c r="D42" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="32"/>
-      <c r="F42" s="30">
+      <c r="E42" s="18"/>
+      <c r="F42" s="15">
         <v>24</v>
       </c>
-      <c r="G42" s="30">
+      <c r="G42" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="33" t="s">
+    <row r="43" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="32" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="30">
+      <c r="E43" s="18"/>
+      <c r="F43" s="15">
         <v>15</v>
       </c>
-      <c r="G43" s="30">
+      <c r="G43" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="33" t="s">
+    <row r="44" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="32" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="30">
+      <c r="E44" s="18"/>
+      <c r="F44" s="15">
         <v>0</v>
       </c>
-      <c r="G44" s="30">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="33" t="s">
+      <c r="G44" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="32" t="s">
+      <c r="C45" s="16"/>
+      <c r="D45" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="30">
+      <c r="E45" s="18"/>
+      <c r="F45" s="15">
         <v>0</v>
       </c>
-      <c r="G45" s="30">
+      <c r="G45" s="15">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="33" t="s">
+    <row r="46" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="33"/>
-      <c r="D46" s="32" t="s">
+      <c r="C46" s="16"/>
+      <c r="D46" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="30">
-        <v>18</v>
-      </c>
-      <c r="G46" s="30">
+      <c r="E46" s="18"/>
+      <c r="F46" s="15">
+        <v>18</v>
+      </c>
+      <c r="G46" s="15">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="A31:P31"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="A32:P32"/>
+    <mergeCell ref="A33:P33"/>
+    <mergeCell ref="A34:P34"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="A36:P36"/>
+    <mergeCell ref="A37:P37"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
@@ -3321,28 +3343,6 @@
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A30:P30"/>
-    <mergeCell ref="A32:P32"/>
-    <mergeCell ref="A33:P33"/>
-    <mergeCell ref="A34:P34"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="A35:P35"/>
-    <mergeCell ref="A36:P36"/>
-    <mergeCell ref="A37:P37"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A29:P29"/>
-    <mergeCell ref="A31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>